<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@2c6d879fda88164f1a9668e233868fd510fd5287 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-care-experience-preference.xlsx
+++ b/StructureDefinition-us-core-care-experience-preference.xlsx
@@ -537,7 +537,7 @@
 </t>
   </si>
   <si>
-    <t>(USCDI) Care Experience Preferences Codes (extensible)</t>
+    <t>(USCDI) Care experience preferences code</t>
   </si>
   <si>
     <t>Describes what was observed. Sometimes this is called the observation "name".</t>
@@ -552,7 +552,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1115.11</t>
+    <t>http://www.fhir.org/guides/uscdi4-sandbox/ValueSet/uscore-care-experience-preference</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -1666,7 +1666,7 @@
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="175.1796875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="67.3671875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="81.89453125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="14.109375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="1.04296875" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@2c2b8f0fb7e0575e4bd36d1c9a5c6ba81cd005fb 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-care-experience-preference.xlsx
+++ b/StructureDefinition-us-core-care-experience-preference.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-11</t>
+    <t>2023-10-12</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1228,7 +1228,7 @@
 </t>
   </si>
   <si>
-    <t>𝗔𝗗𝗗'𝗟 𝗨𝗦𝗖𝗗𝗜: US Core Profiles or other resource the observation is made from</t>
+    <t>𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜: US Core Profiles or other resource the observation is made from</t>
   </si>
   <si>
     <t>US Core Observations, DocumentReference, QuestionnaireResponse or other resource from which this observation value is derived.</t>

</xml_diff>